<commit_message>
fixed bugs with classifier
</commit_message>
<xml_diff>
--- a/Magic_Card_Catalog.xlsx
+++ b/Magic_Card_Catalog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\corey\Documents\Github\mtg_card_classifier\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9084B7D5-29A4-460B-A391-E205AE89828C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{323503D8-61EC-42EB-9BB2-7DB50763CC07}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2295" yWindow="2295" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="844" uniqueCount="291">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="853" uniqueCount="294">
   <si>
     <t>Name</t>
   </si>
@@ -893,6 +893,15 @@
   </si>
   <si>
     <t>Worldsoul Colossus</t>
+  </si>
+  <si>
+    <t>Worm Token</t>
+  </si>
+  <si>
+    <t>Warrior Token</t>
+  </si>
+  <si>
+    <t>Sphinx Insight</t>
   </si>
 </sst>
 </file>
@@ -1237,9 +1246,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:D281"/>
+  <dimension ref="A1:D284"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A263" workbookViewId="0">
+      <selection activeCell="G280" sqref="G280"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -5177,6 +5188,48 @@
         <v>6</v>
       </c>
     </row>
+    <row r="282" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A282" s="4" t="s">
+        <v>291</v>
+      </c>
+      <c r="B282" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C282" s="6">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="D282" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="283" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A283" s="4" t="s">
+        <v>292</v>
+      </c>
+      <c r="B283" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C283" s="6">
+        <v>0.04</v>
+      </c>
+      <c r="D283" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="284" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A284" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="B284" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C284" s="6">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="D284" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>